<commit_message>
Converted data to new format.
</commit_message>
<xml_diff>
--- a/data/Sources/Maffei2.xlsx
+++ b/data/Sources/Maffei2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="245">
   <si>
     <t>From new raw data</t>
   </si>
@@ -743,6 +743,12 @@
   </si>
   <si>
     <t>http://ned.ipac.caltech.edu/cgi-bin/datasearch?objname=maffei+2&amp;meas_type=bot&amp;ebars_spec=ebars&amp;label_spec=no&amp;x_spec=freq&amp;y_spec=Fnu_jy&amp;xr=-1&amp;of=table&amp;search_type=Photometry</t>
+  </si>
+  <si>
+    <t>Freq (Hz)</t>
+  </si>
+  <si>
+    <t>SED (Jy)</t>
   </si>
 </sst>
 </file>
@@ -818,13 +824,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>421279</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>7163</xdr:rowOff>
@@ -1148,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:Q59"/>
+  <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1159,2294 +1165,2593 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:21">
+      <c r="A1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="2">
+        <v>379000000000000</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:21">
+      <c r="A3" s="2">
+        <v>240000000000000</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:21">
+      <c r="A4" s="2">
+        <v>240000000000000</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.67</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:21">
+      <c r="A5" s="2">
+        <v>240000000000000</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.74</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:21">
+      <c r="A6" s="2">
+        <v>240000000000000</v>
+      </c>
+      <c r="B6" s="2">
+        <v>8.4900000000000003E-2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:21">
+      <c r="A7" s="2">
+        <v>182000000000000</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4.67</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="1" t="s">
+    <row r="8" spans="1:21">
+      <c r="A8" s="2">
+        <v>182000000000000</v>
+      </c>
+      <c r="B8" s="2">
+        <v>5.01</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="2">
+        <v>182000000000000</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5.17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="2">
+        <v>182000000000000</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.191</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="1" t="s">
+    <row r="11" spans="1:21">
+      <c r="A11" s="2">
+        <v>138000000000000</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4.92</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="2">
+        <v>138000000000000</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5.28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="2">
+        <v>138000000000000</v>
+      </c>
+      <c r="B13" s="2">
+        <v>5.47</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="2">
+        <v>138000000000000</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="1" t="s">
+    <row r="15" spans="1:21">
+      <c r="A15" s="2">
+        <v>30000000000000</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="2">
+        <v>29700000000000</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.06</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="Q16" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="U16" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="1">
+    <row r="17" spans="1:21">
+      <c r="A17" s="2">
+        <v>25000000000000</v>
+      </c>
+      <c r="B17" s="2">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C17" s="1">
+      <c r="G17" s="1">
         <v>-11.95</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F17" s="2">
+      <c r="J17" s="2">
         <v>456000000000000</v>
       </c>
-      <c r="G17" s="2">
+      <c r="K17" s="2">
         <v>112000000000</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="T17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="U17" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="1">
+    <row r="18" spans="1:21">
+      <c r="A18" s="2">
+        <v>25000000000000</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3.62</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1">
         <v>2</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="1">
+      <c r="G18" s="1">
         <v>9.2899999999999991</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F18" s="2">
+      <c r="J18" s="2">
         <v>379000000000000</v>
       </c>
-      <c r="G18" s="2">
+      <c r="K18" s="2">
         <v>0.49</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="M18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N18" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="1">
+    <row r="19" spans="1:21">
+      <c r="A19" s="2">
+        <v>12000000000000</v>
+      </c>
+      <c r="B19" s="2">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1">
         <v>3</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C19" s="1">
+      <c r="G19" s="1">
         <v>7.024</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F19" s="2">
+      <c r="J19" s="2">
         <v>240000000000000</v>
       </c>
-      <c r="G19" s="2">
+      <c r="K19" s="2">
         <v>2.4700000000000002</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="M19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="Q19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="R19" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="S19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="T19" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="U19" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="1">
+    <row r="20" spans="1:21">
+      <c r="A20" s="2">
+        <v>12000000000000</v>
+      </c>
+      <c r="B20" s="2">
+        <v>9.24</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1">
         <v>4</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C20" s="1">
+      <c r="G20" s="1">
         <v>6.94</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F20" s="2">
+      <c r="J20" s="2">
         <v>240000000000000</v>
       </c>
-      <c r="G20" s="2">
+      <c r="K20" s="2">
         <v>2.67</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="M20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="T20" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="U20" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="1">
+    <row r="21" spans="1:21">
+      <c r="A21" s="2">
+        <v>5000000000000</v>
+      </c>
+      <c r="B21" s="2">
+        <v>135</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1">
         <v>5</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C21" s="1">
+      <c r="G21" s="1">
         <v>6.91</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F21" s="2">
+      <c r="J21" s="2">
         <v>240000000000000</v>
       </c>
-      <c r="G21" s="2">
+      <c r="K21" s="2">
         <v>2.74</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="M21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N21" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="P21" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="S21" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="U21" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="1">
+    <row r="22" spans="1:21">
+      <c r="A22" s="2">
+        <v>5000000000000</v>
+      </c>
+      <c r="B22" s="2">
+        <v>94.8</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1">
         <v>6</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C22" s="1">
+      <c r="G22" s="1">
         <v>10.683</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F22" s="2">
+      <c r="J22" s="2">
         <v>240000000000000</v>
       </c>
-      <c r="G22" s="2">
+      <c r="K22" s="2">
         <v>8.4900000000000003E-2</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="M22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="U22" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="1">
+    <row r="23" spans="1:21">
+      <c r="A23" s="2">
+        <v>3000000000000</v>
+      </c>
+      <c r="B23" s="2">
+        <v>225</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1">
         <v>7</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="1">
+      <c r="G23" s="1">
         <v>5.8520000000000003</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F23" s="2">
+      <c r="J23" s="2">
         <v>182000000000000</v>
       </c>
-      <c r="G23" s="2">
+      <c r="K23" s="2">
         <v>4.67</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J23" s="1" t="s">
+      <c r="M23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="P23" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="S23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="T23" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="U23" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="1">
-        <v>8</v>
-      </c>
-      <c r="B24" s="1" t="s">
+    <row r="24" spans="1:21">
+      <c r="A24" s="2">
+        <v>857000000000</v>
+      </c>
+      <c r="B24" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="1">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C24" s="1">
+      <c r="G24" s="1">
         <v>5.7759999999999998</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F24" s="2">
+      <c r="J24" s="2">
         <v>182000000000000</v>
       </c>
-      <c r="G24" s="2">
+      <c r="K24" s="2">
         <v>5.01</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="M24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="P24" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="Q24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="R24" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="S24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="T24" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="U24" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="1">
+    <row r="25" spans="1:21">
+      <c r="A25" s="2">
+        <v>231000000000</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1">
         <v>9</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C25" s="1">
+      <c r="G25" s="1">
         <v>5.742</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F25" s="2">
+      <c r="J25" s="2">
         <v>182000000000000</v>
       </c>
-      <c r="G25" s="2">
+      <c r="K25" s="2">
         <v>5.17</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J25" s="1" t="s">
+      <c r="M25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="S25" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="T25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="U25" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="1">
+    <row r="26" spans="1:21">
+      <c r="A26" s="2">
+        <v>4850000000</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1">
         <v>10</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C26" s="1">
+      <c r="G26" s="1">
         <v>9.3209999999999997</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F26" s="2">
+      <c r="J26" s="2">
         <v>182000000000000</v>
       </c>
-      <c r="G26" s="2">
+      <c r="K26" s="2">
         <v>0.191</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J26" s="1" t="s">
+      <c r="M26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N26" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="P26" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="Q26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="R26" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="S26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P26" s="1" t="s">
+      <c r="T26" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="U26" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="1">
+    <row r="27" spans="1:21">
+      <c r="A27" s="2">
+        <v>4850000000</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1">
         <v>11</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C27" s="1">
+      <c r="G27" s="1">
         <v>5.3310000000000004</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F27" s="2">
+      <c r="J27" s="2">
         <v>138000000000000</v>
       </c>
-      <c r="G27" s="2">
+      <c r="K27" s="2">
         <v>4.92</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J27" s="1" t="s">
+      <c r="M27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="P27" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="R27" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="S27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="T27" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="U27" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
-      <c r="A28" s="1">
+    <row r="28" spans="1:21">
+      <c r="A28" s="2">
+        <v>1400000000</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1.02</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="1">
         <v>12</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C28" s="1">
+      <c r="G28" s="1">
         <v>5.2539999999999996</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F28" s="2">
+      <c r="J28" s="2">
         <v>138000000000000</v>
       </c>
-      <c r="G28" s="2">
+      <c r="K28" s="2">
         <v>5.28</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J28" s="1" t="s">
+      <c r="M28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="R28" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="S28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="U28" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
-      <c r="A29" s="1">
+    <row r="29" spans="1:21">
+      <c r="A29" s="2">
+        <v>1400000000</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1">
         <v>13</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C29" s="1">
+      <c r="G29" s="1">
         <v>5.2149999999999999</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F29" s="2">
+      <c r="J29" s="2">
         <v>138000000000000</v>
       </c>
-      <c r="G29" s="2">
+      <c r="K29" s="2">
         <v>5.47</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J29" s="1" t="s">
+      <c r="M29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N29" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="P29" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="Q29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="S29" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="T29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="U29" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="1">
+    <row r="30" spans="1:21">
+      <c r="A30" s="2">
+        <v>365000000</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="1">
         <v>14</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C30" s="1">
+      <c r="G30" s="1">
         <v>8.609</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F30" s="2">
+      <c r="J30" s="2">
         <v>138000000000000</v>
       </c>
-      <c r="G30" s="2">
+      <c r="K30" s="2">
         <v>0.24</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J30" s="1" t="s">
+      <c r="M30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N30" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="P30" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="S30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="T30" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="U30" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
-      <c r="A31" s="1">
+    <row r="31" spans="1:21">
+      <c r="A31" s="2">
+        <v>37800000</v>
+      </c>
+      <c r="B31" s="2">
+        <v>5.7</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1">
         <v>15</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C31" s="1">
+      <c r="G31" s="1">
         <v>0.18</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="2">
+      <c r="J31" s="2">
         <v>30000000000000</v>
       </c>
-      <c r="G31" s="2">
+      <c r="K31" s="2">
         <v>0.18</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J31" s="1" t="s">
+      <c r="M31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="S31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="T31" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="U31" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
-      <c r="A32" s="1">
+    <row r="32" spans="1:21">
+      <c r="A32" s="2">
+        <v>37800000</v>
+      </c>
+      <c r="B32" s="2">
+        <v>8.4</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1">
         <v>16</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C32" s="1">
+      <c r="G32" s="1">
         <v>1060</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="2">
+      <c r="J32" s="2">
         <v>29700000000000</v>
       </c>
-      <c r="G32" s="2">
+      <c r="K32" s="2">
         <v>1.06</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J32" s="1" t="s">
+      <c r="M32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N32" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="S32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P32" s="1" t="s">
+      <c r="T32" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="U32" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
-      <c r="A33" s="1">
+    <row r="33" spans="5:21">
+      <c r="E33" s="1">
         <v>17</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="1">
+      <c r="G33" s="1">
         <v>13</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="2">
+      <c r="J33" s="2">
         <v>25000000000000</v>
       </c>
-      <c r="G33" s="2">
+      <c r="K33" s="2">
         <v>13</v>
       </c>
-      <c r="I33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J33" s="1" t="s">
+      <c r="M33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L33" s="3">
+      <c r="P33" s="3">
         <v>0</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="Q33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="S33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P33" s="1" t="s">
+      <c r="T33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q33" s="1" t="s">
+      <c r="U33" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
-      <c r="A34" s="1">
+    <row r="34" spans="5:21">
+      <c r="E34" s="1">
         <v>18</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C34" s="1">
+      <c r="G34" s="1">
         <v>3.6240000000000001</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="2">
+      <c r="J34" s="2">
         <v>25000000000000</v>
       </c>
-      <c r="G34" s="2">
+      <c r="K34" s="2">
         <v>3.62</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="I34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J34" s="1" t="s">
+      <c r="M34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N34" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="O34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="Q34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="R34" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="S34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P34" s="1" t="s">
+      <c r="T34" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="U34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
-      <c r="A35" s="1">
+    <row r="35" spans="5:21">
+      <c r="E35" s="1">
         <v>19</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C35" s="1">
+      <c r="G35" s="1">
         <v>25</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F35" s="2">
+      <c r="J35" s="2">
         <v>12000000000000</v>
       </c>
-      <c r="G35" s="2">
+      <c r="K35" s="2">
         <v>25</v>
       </c>
-      <c r="I35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J35" s="1" t="s">
+      <c r="M35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N35" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="P35" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="Q35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="S35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="U35" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
-      <c r="A36" s="1">
+    <row r="36" spans="5:21">
+      <c r="E36" s="1">
         <v>20</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C36" s="1">
+      <c r="G36" s="1">
         <v>9.2379999999999995</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="2">
+      <c r="J36" s="2">
         <v>12000000000000</v>
       </c>
-      <c r="G36" s="2">
+      <c r="K36" s="2">
         <v>9.24</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J36" s="1" t="s">
+      <c r="M36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N36" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="P36" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="Q36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="R36" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="O36" s="1" t="s">
+      <c r="S36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P36" s="1" t="s">
+      <c r="T36" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="Q36" s="1" t="s">
+      <c r="U36" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
-      <c r="A37" s="1">
+    <row r="37" spans="5:21">
+      <c r="E37" s="1">
         <v>21</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C37" s="1">
+      <c r="G37" s="1">
         <v>135</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="2">
+      <c r="J37" s="2">
         <v>5000000000000</v>
       </c>
-      <c r="G37" s="2">
+      <c r="K37" s="2">
         <v>135</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J37" s="1" t="s">
+      <c r="M37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N37" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="O37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="P37" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="Q37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O37" s="1" t="s">
+      <c r="S37" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P37" s="1" t="s">
+      <c r="T37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q37" s="1" t="s">
+      <c r="U37" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
-      <c r="A38" s="1">
+    <row r="38" spans="5:21">
+      <c r="E38" s="1">
         <v>22</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="1">
+      <c r="G38" s="1">
         <v>94.8</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="2">
+      <c r="J38" s="2">
         <v>5000000000000</v>
       </c>
-      <c r="G38" s="2">
+      <c r="K38" s="2">
         <v>94.8</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J38" s="1" t="s">
+      <c r="M38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N38" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="P38" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="Q38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O38" s="1" t="s">
+      <c r="S38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="P38" s="1" t="s">
+      <c r="T38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q38" s="1" t="s">
+      <c r="U38" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
-      <c r="A39" s="1">
+    <row r="39" spans="5:21">
+      <c r="E39" s="1">
         <v>23</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C39" s="2">
+      <c r="G39" s="2">
         <v>5.3000000000000001E-15</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F39" s="2">
+      <c r="J39" s="2">
         <v>4760000000000</v>
       </c>
-      <c r="G39" s="2">
+      <c r="K39" s="2">
         <v>530000000000</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="M39" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="N39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="P39" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="Q39" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O39" s="1" t="s">
+      <c r="S39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P39" s="1" t="s">
+      <c r="T39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q39" s="1" t="s">
+      <c r="U39" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
-      <c r="A40" s="1">
+    <row r="40" spans="5:21">
+      <c r="E40" s="1">
         <v>24</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="2">
+      <c r="G40" s="2">
         <v>5.1200000000000004E-15</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F40" s="2">
+      <c r="J40" s="2">
         <v>4760000000000</v>
       </c>
-      <c r="G40" s="2">
+      <c r="K40" s="2">
         <v>512000000000</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="M40" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="N40" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="O40" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L40" s="1" t="s">
+      <c r="P40" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="Q40" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O40" s="1" t="s">
+      <c r="S40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="T40" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q40" s="1" t="s">
+      <c r="U40" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
-      <c r="A41" s="1">
+    <row r="41" spans="5:21">
+      <c r="E41" s="1">
         <v>25</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="2">
+      <c r="G41" s="2">
         <v>1.4999999999999999E-15</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F41" s="2">
+      <c r="J41" s="2">
         <v>3410000000000</v>
       </c>
-      <c r="G41" s="2">
+      <c r="K41" s="2">
         <v>150000000000</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="M41" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="N41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="O41" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="P41" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="Q41" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O41" s="1" t="s">
+      <c r="S41" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P41" s="1" t="s">
+      <c r="T41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q41" s="1" t="s">
+      <c r="U41" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
-      <c r="A42" s="1">
+    <row r="42" spans="5:21">
+      <c r="E42" s="1">
         <v>26</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="1">
+      <c r="G42" s="1">
         <v>225</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="2">
+      <c r="J42" s="2">
         <v>3000000000000</v>
       </c>
-      <c r="G42" s="2">
+      <c r="K42" s="2">
         <v>225</v>
       </c>
-      <c r="I42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J42" s="1" t="s">
+      <c r="M42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N42" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="O42" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L42" s="1" t="s">
+      <c r="P42" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="Q42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O42" s="1" t="s">
+      <c r="S42" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P42" s="1" t="s">
+      <c r="T42" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q42" s="1" t="s">
+      <c r="U42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
-      <c r="A43" s="1">
+    <row r="43" spans="5:21">
+      <c r="E43" s="1">
         <v>27</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C43" s="2">
+      <c r="G43" s="2">
         <v>1.4999999999999999E-15</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F43" s="2">
+      <c r="J43" s="2">
         <v>2460000000000</v>
       </c>
-      <c r="G43" s="2">
+      <c r="K43" s="2">
         <v>150000000000</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="L43" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="M43" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="N43" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="O43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="P43" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="Q43" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O43" s="1" t="s">
+      <c r="S43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P43" s="1" t="s">
+      <c r="T43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q43" s="1" t="s">
+      <c r="U43" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
-      <c r="A44" s="1">
+    <row r="44" spans="5:21">
+      <c r="E44" s="1">
         <v>28</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="2">
+      <c r="G44" s="2">
         <v>5.0000000000000004E-16</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F44" s="2">
+      <c r="J44" s="2">
         <v>2070000000000</v>
       </c>
-      <c r="G44" s="2">
+      <c r="K44" s="2">
         <v>50000000000</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="L44" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="M44" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="P44" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="Q44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O44" s="1" t="s">
+      <c r="S44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P44" s="1" t="s">
+      <c r="T44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q44" s="1" t="s">
+      <c r="U44" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
-      <c r="A45" s="1">
+    <row r="45" spans="5:21">
+      <c r="E45" s="1">
         <v>29</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="2">
+      <c r="G45" s="2">
         <v>7.1E-16</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F45" s="2">
+      <c r="J45" s="2">
         <v>2070000000000</v>
       </c>
-      <c r="G45" s="2">
+      <c r="K45" s="2">
         <v>71000000000</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="L45" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="M45" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="N45" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="O45" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="P45" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="M45" s="1" t="s">
+      <c r="Q45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O45" s="1" t="s">
+      <c r="S45" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P45" s="1" t="s">
+      <c r="T45" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q45" s="1" t="s">
+      <c r="U45" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
-      <c r="A46" s="1">
+    <row r="46" spans="5:21">
+      <c r="E46" s="1">
         <v>30</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C46" s="2">
+      <c r="G46" s="2">
         <v>1.21E-14</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F46" s="2">
+      <c r="J46" s="2">
         <v>1900000000000</v>
       </c>
-      <c r="G46" s="2">
+      <c r="K46" s="2">
         <v>1210000000000</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="L46" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="M46" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="N46" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="O46" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="P46" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="Q46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O46" s="1" t="s">
+      <c r="S46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P46" s="1" t="s">
+      <c r="T46" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q46" s="1" t="s">
+      <c r="U46" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
-      <c r="A47" s="1">
+    <row r="47" spans="5:21">
+      <c r="E47" s="1">
         <v>31</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="2">
+      <c r="G47" s="2">
         <v>1.0720000000000001E-14</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F47" s="2">
+      <c r="J47" s="2">
         <v>1900000000000</v>
       </c>
-      <c r="G47" s="2">
+      <c r="K47" s="2">
         <v>1070000000000</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="M47" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="O47" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="P47" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="Q47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O47" s="1" t="s">
+      <c r="S47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P47" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q47" s="1" t="s">
+      <c r="U47" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
-      <c r="A48" s="1">
+    <row r="48" spans="5:21">
+      <c r="E48" s="1">
         <v>32</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C48" s="1">
+      <c r="G48" s="1">
         <v>8.5</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="2">
+      <c r="J48" s="2">
         <v>857000000000</v>
       </c>
-      <c r="G48" s="2">
+      <c r="K48" s="2">
         <v>8.5</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="L48" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J48" s="1" t="s">
+      <c r="M48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N48" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="O48" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="P48" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M48" s="1" t="s">
+      <c r="Q48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O48" s="1" t="s">
+      <c r="S48" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P48" s="1" t="s">
+      <c r="T48" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q48" s="1" t="s">
+      <c r="U48" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
-      <c r="A49" s="1">
+    <row r="49" spans="5:21">
+      <c r="E49" s="1">
         <v>33</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="1">
+      <c r="G49" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F49" s="2">
+      <c r="J49" s="2">
         <v>231000000000</v>
       </c>
-      <c r="G49" s="2">
+      <c r="K49" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="L49" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I49" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J49" s="1" t="s">
+      <c r="M49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N49" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="O49" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="P49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M49" s="1" t="s">
+      <c r="Q49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O49" s="1" t="s">
+      <c r="S49" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P49" s="1" t="s">
+      <c r="T49" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q49" s="1" t="s">
+      <c r="U49" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
-      <c r="A50" s="1">
+    <row r="50" spans="5:21">
+      <c r="E50" s="1">
         <v>34</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="1">
+      <c r="G50" s="1">
         <v>10.9</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F50" s="2">
+      <c r="J50" s="2">
         <v>109000000000</v>
       </c>
-      <c r="G50" s="2">
+      <c r="K50" s="2">
         <v>3970000</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="M50" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="N50" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="O50" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="P50" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="M50" s="1" t="s">
+      <c r="Q50" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N50" s="1" t="s">
+      <c r="R50" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="O50" s="1" t="s">
+      <c r="S50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P50" s="1" t="s">
+      <c r="T50" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q50" s="1" t="s">
+      <c r="U50" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
-      <c r="A51" s="1">
+    <row r="51" spans="5:21">
+      <c r="E51" s="1">
         <v>35</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C51" s="1">
+      <c r="G51" s="1">
         <v>243</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F51" s="2">
+      <c r="J51" s="2">
         <v>4850000000</v>
       </c>
-      <c r="G51" s="2">
+      <c r="K51" s="2">
         <v>0.24299999999999999</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I51" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J51" s="1" t="s">
+      <c r="M51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N51" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="O51" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L51" s="1" t="s">
+      <c r="P51" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M51" s="1" t="s">
+      <c r="Q51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N51" s="1" t="s">
+      <c r="R51" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O51" s="1" t="s">
+      <c r="S51" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="P51" s="1" t="s">
+      <c r="T51" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q51" s="1" t="s">
+      <c r="U51" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
-      <c r="A52" s="1">
+    <row r="52" spans="5:21">
+      <c r="E52" s="1">
         <v>36</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="1">
+      <c r="G52" s="1">
         <v>375</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F52" s="2">
+      <c r="J52" s="2">
         <v>4850000000</v>
       </c>
-      <c r="G52" s="2">
+      <c r="K52" s="2">
         <v>0.375</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="L52" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I52" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J52" s="1" t="s">
+      <c r="M52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N52" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="O52" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L52" s="1" t="s">
+      <c r="P52" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M52" s="1" t="s">
+      <c r="Q52" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N52" s="1" t="s">
+      <c r="R52" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O52" s="1" t="s">
+      <c r="S52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P52" s="1" t="s">
+      <c r="T52" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q52" s="1" t="s">
+      <c r="U52" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
-      <c r="A53" s="1">
+    <row r="53" spans="5:21">
+      <c r="E53" s="1">
         <v>37</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="1">
+      <c r="G53" s="1">
         <v>11.15</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F53" s="2">
+      <c r="J53" s="2">
         <v>1420000000</v>
       </c>
-      <c r="G53" s="2">
+      <c r="K53" s="2">
         <v>1510000</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="L53" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="M53" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="N53" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="O53" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L53" s="1" t="s">
+      <c r="P53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M53" s="1" t="s">
+      <c r="Q53" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N53" s="1" t="s">
+      <c r="R53" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O53" s="1" t="s">
+      <c r="S53" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P53" s="1" t="s">
+      <c r="T53" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q53" s="1" t="s">
+      <c r="U53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
-      <c r="A54" s="1">
+    <row r="54" spans="5:21">
+      <c r="E54" s="1">
         <v>38</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="1">
+      <c r="G54" s="1">
         <v>93</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="I54" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F54" s="2">
+      <c r="J54" s="2">
         <v>1420000000</v>
       </c>
-      <c r="G54" s="2">
+      <c r="K54" s="2">
         <v>439000</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="L54" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="M54" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J54" s="1" t="s">
+      <c r="N54" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="O54" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L54" s="1" t="s">
+      <c r="P54" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M54" s="1" t="s">
+      <c r="Q54" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N54" s="1" t="s">
+      <c r="R54" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O54" s="1" t="s">
+      <c r="S54" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P54" s="1" t="s">
+      <c r="T54" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q54" s="1" t="s">
+      <c r="U54" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
-      <c r="A55" s="1">
+    <row r="55" spans="5:21">
+      <c r="E55" s="1">
         <v>39</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C55" s="1">
+      <c r="G55" s="1">
         <v>1015</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="I55" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F55" s="2">
+      <c r="J55" s="2">
         <v>1400000000</v>
       </c>
-      <c r="G55" s="2">
+      <c r="K55" s="2">
         <v>1.02</v>
       </c>
-      <c r="I55" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J55" s="1" t="s">
+      <c r="M55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N55" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="O55" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L55" s="1" t="s">
+      <c r="P55" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M55" s="1" t="s">
+      <c r="Q55" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N55" s="1" t="s">
+      <c r="R55" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O55" s="1" t="s">
+      <c r="S55" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P55" s="1" t="s">
+      <c r="T55" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q55" s="1" t="s">
+      <c r="U55" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
-      <c r="A56" s="1">
+    <row r="56" spans="5:21">
+      <c r="E56" s="1">
         <v>40</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="1">
+      <c r="G56" s="1">
         <v>286.2</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="H56" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="I56" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F56" s="2">
+      <c r="J56" s="2">
         <v>1400000000</v>
       </c>
-      <c r="G56" s="2">
+      <c r="K56" s="2">
         <v>0.28599999999999998</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="L56" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I56" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J56" s="1" t="s">
+      <c r="M56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N56" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="O56" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L56" s="1" t="s">
+      <c r="P56" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M56" s="1" t="s">
+      <c r="Q56" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N56" s="1" t="s">
+      <c r="R56" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O56" s="1" t="s">
+      <c r="S56" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P56" s="1" t="s">
+      <c r="T56" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q56" s="1" t="s">
+      <c r="U56" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
-      <c r="A57" s="1">
+    <row r="57" spans="5:21">
+      <c r="E57" s="1">
         <v>41</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="1">
+      <c r="G57" s="1">
         <v>0.42899999999999999</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="I57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F57" s="2">
+      <c r="J57" s="2">
         <v>365000000</v>
       </c>
-      <c r="G57" s="2">
+      <c r="K57" s="2">
         <v>0.42899999999999999</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="L57" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I57" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J57" s="1" t="s">
+      <c r="M57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N57" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K57" s="1" t="s">
+      <c r="O57" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L57" s="1" t="s">
+      <c r="P57" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M57" s="1" t="s">
+      <c r="Q57" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N57" s="1" t="s">
+      <c r="R57" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O57" s="1" t="s">
+      <c r="S57" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P57" s="1" t="s">
+      <c r="T57" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q57" s="1" t="s">
+      <c r="U57" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
-      <c r="A58" s="1">
+    <row r="58" spans="5:21">
+      <c r="E58" s="1">
         <v>42</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="1">
+      <c r="G58" s="1">
         <v>5.7</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="H58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="I58" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F58" s="2">
+      <c r="J58" s="2">
         <v>37800000</v>
       </c>
-      <c r="G58" s="2">
+      <c r="K58" s="2">
         <v>5.7</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="L58" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I58" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J58" s="1" t="s">
+      <c r="M58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N58" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="O58" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L58" s="1" t="s">
+      <c r="P58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M58" s="1" t="s">
+      <c r="Q58" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N58" s="1" t="s">
+      <c r="R58" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O58" s="1" t="s">
+      <c r="S58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P58" s="1" t="s">
+      <c r="T58" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q58" s="1" t="s">
+      <c r="U58" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
-      <c r="A59" s="1">
+    <row r="59" spans="5:21">
+      <c r="E59" s="1">
         <v>43</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="1">
+      <c r="G59" s="1">
         <v>8.4</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="H59" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="I59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F59" s="2">
+      <c r="J59" s="2">
         <v>37800000</v>
       </c>
-      <c r="G59" s="2">
+      <c r="K59" s="2">
         <v>8.4</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="L59" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I59" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J59" s="1" t="s">
+      <c r="M59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N59" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="O59" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L59" s="1" t="s">
+      <c r="P59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M59" s="1" t="s">
+      <c r="Q59" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N59" s="1" t="s">
+      <c r="R59" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O59" s="1" t="s">
+      <c r="S59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P59" s="1" t="s">
+      <c r="T59" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q59" s="1" t="s">
+      <c r="U59" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q3" r:id="rId1"/>
+    <hyperlink ref="U3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>